<commit_message>
Edits text to be clearer on FY versus CY. Slightly edits files to make data layout consistent.
</commit_message>
<xml_diff>
--- a/downloads/federal_revenue_by_company_CY2013_2015-11-10.xlsx
+++ b/downloads/federal_revenue_by_company_CY2013_2015-11-10.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="24960" windowHeight="15060"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15600"/>
   </bookViews>
   <sheets>
     <sheet name="Data Portal with ONRR, BLM, OSM" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Data Portal with ONRR, BLM, OSM'!$A$1:$D$2704</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Data Portal with ONRR, BLM, OSM'!$1:$1</definedName>
   </definedNames>
-  <calcPr calcId="150001" calcOnSave="0" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -3212,10 +3212,10 @@
   <dimension ref="A1:G2705"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2704" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2457" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F76" sqref="F76"/>
+      <selection pane="bottomRight" activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0"/>

</xml_diff>